<commit_message>
adion de un riesgo del proyecto
se realizo un cambio en  eçel docuemnto de riesgo del prpyecto
</commit_message>
<xml_diff>
--- a/ADMINISTRACION/Gestion de Riesgos/MATRIZ Y PLAN DE RIESGO V2.0.xlsx
+++ b/ADMINISTRACION/Gestion de Riesgos/MATRIZ Y PLAN DE RIESGO V2.0.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ESTEBAN\Desktop\ESTEBAN\ADMINISTRACION\Gestion de Riesgos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyecto-SIPRECO_2018\ADMINISTRACION\Gestion de Riesgos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13605" windowHeight="9195" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13605" windowHeight="9195"/>
   </bookViews>
   <sheets>
     <sheet name="Matricez Generales de Riesgo" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="87">
   <si>
     <t>ALTO</t>
   </si>
@@ -280,6 +280,12 @@
   </si>
   <si>
     <t>el cronograma del proyecto no esta actualizado</t>
+  </si>
+  <si>
+    <t>RISK - IR-011</t>
+  </si>
+  <si>
+    <t>la gestion de configuracion no esta definida y por ello se pierden documentaciones en el transcurso del proyecto.</t>
   </si>
 </sst>
 </file>
@@ -500,7 +506,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -545,33 +551,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -584,6 +563,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -894,8 +907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F98"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D94" sqref="D94:D98"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -908,12 +921,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
@@ -1003,13 +1016,13 @@
       <c r="B9" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="36" t="s">
+      <c r="D9" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="36" t="s">
+      <c r="E9" s="27" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1017,13 +1030,13 @@
       <c r="B10" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="36" t="s">
+      <c r="D10" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="36" t="s">
+      <c r="E10" s="27" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1031,13 +1044,13 @@
       <c r="B11" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C11" s="37" t="s">
+      <c r="C11" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="36" t="s">
+      <c r="D11" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="36" t="s">
+      <c r="E11" s="27" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1045,13 +1058,13 @@
       <c r="B12" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C12" s="37" t="s">
+      <c r="C12" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="36" t="s">
+      <c r="D12" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="36" t="s">
+      <c r="E12" s="27" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1059,13 +1072,13 @@
       <c r="B13" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C13" s="37" t="s">
+      <c r="C13" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="36" t="s">
+      <c r="D13" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="38" t="s">
+      <c r="E13" s="29" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1073,12 +1086,12 @@
     <row r="15" spans="2:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="2:5" ht="63.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B57" s="25" t="s">
+      <c r="B57" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="C57" s="26"/>
-      <c r="D57" s="26"/>
-      <c r="E57" s="27"/>
+      <c r="C57" s="32"/>
+      <c r="D57" s="32"/>
+      <c r="E57" s="33"/>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B58" s="6" t="s">
@@ -1168,10 +1181,10 @@
       <c r="B64" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C64" s="38" t="s">
+      <c r="C64" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="D64" s="37" t="s">
+      <c r="D64" s="28" t="s">
         <v>41</v>
       </c>
       <c r="E64" s="23">
@@ -1182,10 +1195,10 @@
       <c r="B65" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C65" s="38" t="s">
+      <c r="C65" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="D65" s="37" t="s">
+      <c r="D65" s="28" t="s">
         <v>41</v>
       </c>
       <c r="E65" s="23">
@@ -1196,10 +1209,10 @@
       <c r="B66" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C66" s="38" t="s">
+      <c r="C66" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="D66" s="37" t="s">
+      <c r="D66" s="28" t="s">
         <v>42</v>
       </c>
       <c r="E66" s="23">
@@ -1210,10 +1223,10 @@
       <c r="B67" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C67" s="36" t="s">
+      <c r="C67" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="D67" s="37" t="s">
+      <c r="D67" s="28" t="s">
         <v>41</v>
       </c>
       <c r="E67" s="23">
@@ -1224,24 +1237,38 @@
       <c r="B68" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C68" s="36" t="s">
+      <c r="C68" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="D68" s="37" t="s">
+      <c r="D68" s="28" t="s">
         <v>42</v>
       </c>
       <c r="E68" s="23">
         <v>43251</v>
       </c>
     </row>
+    <row r="69" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B69" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C69" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="D69" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="E69" s="41">
+        <v>43258</v>
+      </c>
+    </row>
     <row r="73" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B73" s="24" t="s">
+      <c r="B73" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="C73" s="24"/>
-      <c r="D73" s="24"/>
-      <c r="E73" s="24"/>
-      <c r="F73" s="24"/>
+      <c r="C73" s="30"/>
+      <c r="D73" s="30"/>
+      <c r="E73" s="30"/>
+      <c r="F73" s="30"/>
     </row>
     <row r="74" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B74" s="5" t="s">
@@ -1349,16 +1376,16 @@
       <c r="B80" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C80" s="36" t="s">
+      <c r="C80" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="D80" s="37" t="s">
+      <c r="D80" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="E80" s="36" t="s">
+      <c r="E80" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F80" s="36" t="s">
+      <c r="F80" s="27" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1366,16 +1393,16 @@
       <c r="B81" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C81" s="36" t="s">
+      <c r="C81" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="D81" s="37" t="s">
+      <c r="D81" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="E81" s="36" t="s">
+      <c r="E81" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F81" s="36" t="s">
+      <c r="F81" s="27" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1383,16 +1410,16 @@
       <c r="B82" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C82" s="36" t="s">
+      <c r="C82" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="D82" s="37" t="s">
+      <c r="D82" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="E82" s="36" t="s">
+      <c r="E82" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F82" s="36" t="s">
+      <c r="F82" s="27" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1400,16 +1427,16 @@
       <c r="B83" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C83" s="36" t="s">
+      <c r="C83" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="D83" s="37" t="s">
+      <c r="D83" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="E83" s="36" t="s">
+      <c r="E83" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F83" s="36" t="s">
+      <c r="F83" s="27" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1417,39 +1444,39 @@
       <c r="B84" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C84" s="36" t="s">
+      <c r="C84" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="D84" s="37" t="s">
+      <c r="D84" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="E84" s="36" t="s">
+      <c r="E84" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F84" s="36" t="s">
+      <c r="F84" s="27" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="85" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C85" s="33"/>
-      <c r="D85" s="34"/>
-      <c r="E85" s="33"/>
-      <c r="F85" s="35"/>
+      <c r="C85" s="24"/>
+      <c r="D85" s="25"/>
+      <c r="E85" s="24"/>
+      <c r="F85" s="26"/>
     </row>
     <row r="86" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C86" s="33"/>
-      <c r="D86" s="34"/>
-      <c r="E86" s="33"/>
-      <c r="F86" s="35"/>
+      <c r="C86" s="24"/>
+      <c r="D86" s="25"/>
+      <c r="E86" s="24"/>
+      <c r="F86" s="26"/>
     </row>
     <row r="87" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B87" s="25" t="s">
+      <c r="B87" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="C87" s="26"/>
-      <c r="D87" s="26"/>
-      <c r="E87" s="26"/>
-      <c r="F87" s="27"/>
+      <c r="C87" s="32"/>
+      <c r="D87" s="32"/>
+      <c r="E87" s="32"/>
+      <c r="F87" s="33"/>
     </row>
     <row r="88" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B88" s="4" t="s">
@@ -1560,13 +1587,13 @@
       <c r="C94" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D94" s="36" t="s">
+      <c r="D94" s="27" t="s">
         <v>67</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F94" s="36" t="s">
+      <c r="F94" s="27" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1577,13 +1604,13 @@
       <c r="C95" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D95" s="36" t="s">
+      <c r="D95" s="27" t="s">
         <v>68</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F95" s="36" t="s">
+      <c r="F95" s="27" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1594,13 +1621,13 @@
       <c r="C96" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D96" s="36" t="s">
+      <c r="D96" s="27" t="s">
         <v>69</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F96" s="36" t="s">
+      <c r="F96" s="27" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1611,13 +1638,13 @@
       <c r="C97" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D97" s="36" t="s">
+      <c r="D97" s="27" t="s">
         <v>70</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F97" s="36" t="s">
+      <c r="F97" s="27" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1628,13 +1655,13 @@
       <c r="C98" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D98" s="38" t="s">
+      <c r="D98" s="29" t="s">
         <v>76</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F98" s="36" t="s">
+      <c r="F98" s="27" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1653,7 +1680,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -1667,10 +1694,10 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="29"/>
+      <c r="C4" s="35"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="9"/>
@@ -1704,13 +1731,13 @@
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="12"/>
-      <c r="C10" s="36" t="s">
+      <c r="C10" s="27" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="9"/>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="27" t="s">
         <v>68</v>
       </c>
       <c r="D11" s="16" t="s">
@@ -1721,20 +1748,20 @@
     </row>
     <row r="12" spans="2:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="10"/>
-      <c r="C12" s="36" t="s">
+      <c r="C12" s="27" t="s">
         <v>69</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="1"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="31"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="37"/>
       <c r="H12" s="19"/>
     </row>
     <row r="13" spans="2:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="21"/>
-      <c r="C13" s="36" t="s">
+      <c r="C13" s="27" t="s">
         <v>70</v>
       </c>
       <c r="D13" s="15" t="s">
@@ -1747,25 +1774,25 @@
     </row>
     <row r="14" spans="2:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="9"/>
-      <c r="C14" s="38" t="s">
+      <c r="C14" s="29" t="s">
         <v>76</v>
       </c>
       <c r="D14" s="15" t="s">
         <v>32</v>
       </c>
       <c r="E14" s="17"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="31"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="37"/>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E15" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F15" s="32" t="s">
+      <c r="F15" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="G15" s="32"/>
+      <c r="G15" s="38"/>
       <c r="H15" s="13" t="s">
         <v>0</v>
       </c>

</xml_diff>